<commit_message>
run experiments & add data to excel
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D37D34-B732-4AB4-A60A-3AE1593CE172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A86FA4E-8FDB-423F-9180-BA0EAEF70050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
@@ -136,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,9 +164,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1256,7 +1263,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1582,17 +1589,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5605-5B40-4E95-A326-20DE76CB0444}">
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:X98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="14.6640625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="14.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
     <col min="8" max="11" width="11.5546875" style="4" customWidth="1"/>
     <col min="12" max="15" width="16.44140625" style="6" customWidth="1"/>
@@ -1612,11 +1621,11 @@
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="8" t="s">
@@ -1653,10 +1662,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
       <c r="C2" s="3">
@@ -1666,10 +1675,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="3">
+        <f>D2-1</f>
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <f>D2-1</f>
         <v>1</v>
       </c>
       <c r="H2" s="5">
@@ -1683,11 +1692,11 @@
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6">
-        <f>((D2-1)-1)*E2</f>
+        <f>((D2-1)-1)*F2</f>
         <v>0</v>
       </c>
       <c r="M2" s="6">
-        <f>(D2-1)*(E2-1)</f>
+        <f>(D2-1)*(F2-1)</f>
         <v>0</v>
       </c>
       <c r="N2" s="6">
@@ -1695,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="6">
-        <f>E2/$B$2</f>
+        <f>F2/$B$2</f>
         <v>1</v>
       </c>
       <c r="P2" s="6" t="str">
@@ -1704,16 +1713,16 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1721,11 +1730,11 @@
         <v>3</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <f>D4-1</f>
+        <v>2</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F3:F60" si="0">D4-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5">
         <v>10.99</v>
@@ -1738,11 +1747,11 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="6">
-        <f>((D4-1)-1)*E4</f>
+        <f>((D4-1)-1)*F4</f>
         <v>1</v>
       </c>
       <c r="M4" s="6">
-        <f>(D4-1)*(E4-1)</f>
+        <f>(D4-1)*(F4-1)</f>
         <v>0</v>
       </c>
       <c r="N4" s="6">
@@ -1750,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" ref="O4:O15" si="1">E4/$B$2</f>
+        <f>F4/$B$2</f>
         <v>1</v>
       </c>
       <c r="P4" s="6" t="str">
@@ -1765,8 +1774,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="3">
         <v>3</v>
       </c>
@@ -1774,11 +1783,11 @@
         <v>5</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <f>D5-1</f>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5">
         <v>10.99</v>
@@ -1791,11 +1800,11 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="6">
-        <f>((D5-1)-1)*E5</f>
+        <f>((D5-1)-1)*F5</f>
         <v>3</v>
       </c>
       <c r="M5" s="6">
-        <f>(D5-1)*(E5-1)</f>
+        <f>(D5-1)*(F5-1)</f>
         <v>0</v>
       </c>
       <c r="N5" s="6">
@@ -1803,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="O5" s="6">
-        <f t="shared" si="1"/>
+        <f>F5/$B$2</f>
         <v>1</v>
       </c>
       <c r="P5" s="6" t="str">
@@ -1812,8 +1821,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1821,11 +1830,11 @@
         <v>9</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <f>D6-1</f>
+        <v>8</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H6" s="5">
         <v>10.99</v>
@@ -1838,11 +1847,11 @@
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="6">
-        <f>((D6-1)-1)*E6</f>
+        <f>((D6-1)-1)*F6</f>
         <v>7</v>
       </c>
       <c r="M6" s="6">
-        <f>(D6-1)*(E6-1)</f>
+        <f>(D6-1)*(F6-1)</f>
         <v>0</v>
       </c>
       <c r="N6" s="6">
@@ -1850,7 +1859,7 @@
         <v>8</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" si="1"/>
+        <f>F6/$B$2</f>
         <v>1</v>
       </c>
       <c r="P6" s="6" t="str">
@@ -1859,8 +1868,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3">
         <v>9</v>
       </c>
@@ -1868,11 +1877,11 @@
         <v>17</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <f>D7-1</f>
+        <v>16</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>10.99</v>
@@ -1885,11 +1894,11 @@
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="6">
-        <f>((D7-1)-1)*E7</f>
+        <f>((D7-1)-1)*F7</f>
         <v>15</v>
       </c>
       <c r="M7" s="6">
-        <f>(D7-1)*(E7-1)</f>
+        <f>(D7-1)*(F7-1)</f>
         <v>0</v>
       </c>
       <c r="N7" s="6">
@@ -1897,7 +1906,7 @@
         <v>16</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" si="1"/>
+        <f>F7/$B$2</f>
         <v>1</v>
       </c>
       <c r="P7" s="6" t="str">
@@ -1909,8 +1918,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3">
         <v>17</v>
       </c>
@@ -1918,11 +1927,11 @@
         <v>33</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <f>D8-1</f>
+        <v>32</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
         <v>10.99</v>
@@ -1935,11 +1944,11 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6">
-        <f>((D8-1)-1)*E8</f>
+        <f>((D8-1)-1)*F8</f>
         <v>31</v>
       </c>
       <c r="M8" s="6">
-        <f>(D8-1)*(E8-1)</f>
+        <f>(D8-1)*(F8-1)</f>
         <v>0</v>
       </c>
       <c r="N8" s="6">
@@ -1947,7 +1956,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="1"/>
+        <f>F8/$B$2</f>
         <v>1</v>
       </c>
       <c r="P8" s="6" t="str">
@@ -1959,16 +1968,16 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="3">
         <v>2</v>
       </c>
@@ -1976,11 +1985,11 @@
         <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>2</v>
+        <f>D10-1</f>
+        <v>1</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="5">
         <v>10.99</v>
@@ -1993,29 +2002,29 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="6">
-        <f>((D10-1)-1)*E10</f>
+        <f t="shared" ref="L10:L15" si="0">((D10-1)-1)*F10</f>
         <v>0</v>
       </c>
       <c r="M10" s="6">
-        <f>(D10-1)*(E10-1)</f>
+        <f t="shared" ref="M10:M15" si="1">(D10-1)*(F10-1)</f>
         <v>1</v>
       </c>
       <c r="N10" s="6">
-        <f>(D10-1)/$B$2</f>
+        <f t="shared" ref="N10:N19" si="2">(D10-1)/$B$2</f>
         <v>1</v>
       </c>
       <c r="O10" s="6">
-        <f t="shared" si="1"/>
+        <f>F10/$B$2</f>
         <v>2</v>
       </c>
       <c r="P10" s="6" t="str">
-        <f t="shared" ref="P10:P15" si="2">IF(L10&lt;M10, "Lino", "Paolo")</f>
+        <f t="shared" ref="P10:P15" si="3">IF(L10&lt;M10, "Lino", "Paolo")</f>
         <v>Lino</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -2023,11 +2032,11 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
+        <f>D11-1</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>4</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H11" s="5">
         <v>10.99</v>
@@ -2040,29 +2049,29 @@
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="6">
-        <f>((D11-1)-1)*E11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M11" s="6">
-        <f>(D11-1)*(E11-1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N11" s="6">
-        <f>(D11-1)/$B$2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O11" s="6">
-        <f t="shared" si="1"/>
+        <f>F11/$B$2</f>
         <v>4</v>
       </c>
       <c r="P11" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3">
         <v>2</v>
       </c>
@@ -2070,11 +2079,11 @@
         <v>2</v>
       </c>
       <c r="E12" s="3">
+        <f>D12-1</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <v>8</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H12" s="5">
         <v>10.99</v>
@@ -2087,29 +2096,29 @@
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="6">
-        <f>((D12-1)-1)*E12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12" s="6">
-        <f>(D12-1)*(E12-1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="N12" s="6">
-        <f>(D12-1)/$B$2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="1"/>
+        <f>F12/$B$2</f>
         <v>8</v>
       </c>
       <c r="P12" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3">
         <v>2</v>
       </c>
@@ -2117,11 +2126,11 @@
         <v>2</v>
       </c>
       <c r="E13" s="3">
+        <f>D13-1</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
         <v>16</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H13" s="5">
         <v>10.99</v>
@@ -2134,29 +2143,29 @@
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="6">
-        <f>((D13-1)-1)*E13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M13" s="6">
-        <f>(D13-1)*(E13-1)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="N13" s="6">
-        <f>(D13-1)/$B$2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="1"/>
+        <f>F13/$B$2</f>
         <v>16</v>
       </c>
       <c r="P13" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3">
         <v>2</v>
       </c>
@@ -2164,11 +2173,11 @@
         <v>2</v>
       </c>
       <c r="E14" s="3">
+        <f>D14-1</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
         <v>24</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H14" s="5">
         <v>10.99</v>
@@ -2181,29 +2190,29 @@
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="6">
-        <f>((D14-1)-1)*E14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M14" s="6">
-        <f>(D14-1)*(E14-1)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="N14" s="6">
-        <f>(D14-1)/$B$2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O14" s="6">
-        <f t="shared" si="1"/>
+        <f>F14/$B$2</f>
         <v>24</v>
       </c>
       <c r="P14" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="3">
         <v>2</v>
       </c>
@@ -2211,11 +2220,11 @@
         <v>2</v>
       </c>
       <c r="E15" s="3">
+        <f>D15-1</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <v>48</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>10.99</v>
@@ -2228,439 +2237,404 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="6">
-        <f>((D15-1)-1)*E15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15" s="6">
-        <f>(D15-1)*(E15-1)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="N15" s="6">
-        <f>(D15-1)/$B$2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="1"/>
+        <f>F15/$B$2</f>
         <v>48</v>
       </c>
       <c r="P15" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10">
-        <v>2</v>
-      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <f>D17-1</f>
+        <v>8</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H17" s="5">
-        <v>22.04</v>
+        <v>10.99</v>
       </c>
       <c r="I17" s="5">
-        <v>21.91</v>
+        <v>1.22</v>
       </c>
       <c r="J17" s="5">
-        <v>21.85</v>
+        <v>1.45</v>
       </c>
       <c r="K17" s="5"/>
-      <c r="N17" s="6">
-        <f>(D17-1)/$B$17</f>
-        <v>0.5</v>
-      </c>
-      <c r="O17" s="6">
-        <f>E17/$B$17</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O17" s="10">
+        <f t="shared" ref="O17:O19" si="4">F17/$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="3">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3">
+        <f>D18-1</f>
+        <v>8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>16</v>
+      </c>
+      <c r="H18" s="5">
+        <v>10.99</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1.45</v>
+      </c>
       <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O18" s="10">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <f>D19-1</f>
+        <v>16</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H19" s="5">
-        <v>22.04</v>
+        <v>10.99</v>
       </c>
       <c r="I19" s="5">
-        <v>11.12</v>
+        <v>1.21</v>
       </c>
       <c r="J19" s="5">
-        <v>11.17</v>
+        <v>0.81</v>
       </c>
       <c r="K19" s="5"/>
-      <c r="N19" s="6">
-        <f>(D19-1)/$B$17</f>
-        <v>1</v>
-      </c>
-      <c r="O19" s="6">
-        <f>E19/$B$17</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="3">
-        <v>3</v>
-      </c>
-      <c r="D20" s="3">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H20" s="5">
-        <v>22.04</v>
-      </c>
-      <c r="I20" s="5">
-        <v>9.91</v>
-      </c>
-      <c r="J20" s="5">
-        <v>5.5209999999999999</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="N20" s="6">
-        <f>(D20-1)/$B$17</f>
-        <v>2</v>
-      </c>
-      <c r="O20" s="6">
-        <f t="shared" ref="O20:O30" si="3">E20/$B$17</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="3">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H21" s="5">
-        <v>22.04</v>
-      </c>
-      <c r="I21" s="5">
-        <v>9.92</v>
-      </c>
-      <c r="J21" s="5">
-        <v>2.81</v>
-      </c>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="N21" s="6">
-        <f>(D21-1)/$B$17</f>
-        <v>4</v>
-      </c>
-      <c r="O21" s="6">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11">
+        <v>2</v>
+      </c>
       <c r="C22" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E22" s="3">
+        <f>D22-1</f>
         <v>1</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
         <v>22.04</v>
       </c>
       <c r="I22" s="5">
-        <v>9.94</v>
+        <v>21.91</v>
       </c>
       <c r="J22" s="5">
-        <v>1.46</v>
+        <v>21.85</v>
       </c>
       <c r="K22" s="5"/>
       <c r="N22" s="6">
-        <f>(D22-1)/$B$17</f>
-        <v>8</v>
+        <f>(D22-1)/$B$22</f>
+        <v>0.5</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="3"/>
+        <f>F22/$B$22</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="3">
-        <v>17</v>
-      </c>
-      <c r="D23" s="3">
-        <v>33</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="H23" s="5">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3">
+        <f>D24-1</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
         <v>22.04</v>
       </c>
-      <c r="I23" s="5">
-        <v>9.92</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0.89</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="N23" s="6">
-        <f>(D23-1)/$B$17</f>
-        <v>16</v>
-      </c>
-      <c r="O23" s="6">
-        <f t="shared" si="3"/>
+      <c r="I24" s="5">
+        <v>11.12</v>
+      </c>
+      <c r="J24" s="5">
+        <v>11.17</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="N24" s="6">
+        <f>(D24-1)/$B$22</f>
+        <v>1</v>
+      </c>
+      <c r="O24" s="6">
+        <f>F24/$B$22</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E25" s="3">
-        <v>2</v>
+        <f>D25-1</f>
+        <v>4</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H25" s="5">
         <v>22.04</v>
       </c>
       <c r="I25" s="5">
-        <v>11.04</v>
+        <v>9.91</v>
       </c>
       <c r="J25" s="5">
-        <v>11</v>
+        <v>5.5209999999999999</v>
       </c>
       <c r="K25" s="5"/>
       <c r="N25" s="6">
-        <f>(D25-1)/$B$17</f>
+        <f>(D25-1)/$B$22</f>
+        <v>2</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" ref="O25:O39" si="5">F25/$B$22</f>
         <v>0.5</v>
       </c>
-      <c r="O25" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E26" s="3">
-        <v>4</v>
+        <f>D26-1</f>
+        <v>8</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H26" s="5">
         <v>22.04</v>
       </c>
       <c r="I26" s="5">
-        <v>4.8</v>
+        <v>9.92</v>
       </c>
       <c r="J26" s="5">
-        <v>11.06</v>
+        <v>2.81</v>
       </c>
       <c r="K26" s="5"/>
       <c r="N26" s="6">
-        <f>(D26-1)/$B$17</f>
+        <f>(D26-1)/$B$22</f>
+        <v>4</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="O26" s="6">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3">
-        <v>8</v>
+        <f>D27-1</f>
+        <v>16</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H27" s="5">
         <v>22.04</v>
       </c>
       <c r="I27" s="5">
-        <v>2.37</v>
+        <v>9.94</v>
       </c>
       <c r="J27" s="5">
-        <v>11.08</v>
+        <v>1.46</v>
       </c>
       <c r="K27" s="5"/>
       <c r="N27" s="6">
-        <f>(D27-1)/$B$17</f>
+        <f>(D27-1)/$B$22</f>
+        <v>8</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="O27" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="E28" s="3">
-        <v>16</v>
+        <f>D28-1</f>
+        <v>32</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H28" s="5">
         <v>22.04</v>
       </c>
       <c r="I28" s="5">
-        <v>1.24</v>
+        <v>9.92</v>
       </c>
       <c r="J28" s="5">
-        <v>11.07</v>
+        <v>0.89</v>
       </c>
       <c r="K28" s="5"/>
       <c r="N28" s="6">
-        <f>(D28-1)/$B$17</f>
+        <f>(D28-1)/$B$22</f>
+        <v>16</v>
+      </c>
+      <c r="O28" s="6">
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="O28" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="E29" s="3">
-        <v>24</v>
-      </c>
-      <c r="F29" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H29" s="5">
-        <v>22.04</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0.86</v>
-      </c>
-      <c r="J29" s="5">
-        <v>11.05</v>
-      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="N29" s="6">
-        <f>(D29-1)/$B$17</f>
-        <v>0.5</v>
-      </c>
-      <c r="O29" s="6">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="10"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3">
         <v>2</v>
       </c>
@@ -2668,43 +2642,69 @@
         <v>2</v>
       </c>
       <c r="E30" s="3">
-        <v>48</v>
+        <f>D30-1</f>
+        <v>1</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5">
         <v>22.04</v>
       </c>
       <c r="I30" s="5">
-        <v>0.49</v>
+        <v>11.04</v>
       </c>
       <c r="J30" s="5">
-        <v>11.07</v>
+        <v>11</v>
       </c>
       <c r="K30" s="5"/>
       <c r="N30" s="6">
-        <f>(D30-1)/$B$17</f>
+        <f t="shared" ref="N30:N39" si="6">(D30-1)/$B$22</f>
         <v>0.5</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <f>D31-1</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>4</v>
+      </c>
+      <c r="H31" s="5">
+        <v>22.04</v>
+      </c>
+      <c r="I31" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="J31" s="5">
+        <v>11.06</v>
+      </c>
       <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10">
-        <v>4</v>
-      </c>
+      <c r="N31" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="O31" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="3">
         <v>2</v>
       </c>
@@ -2712,260 +2712,275 @@
         <v>2</v>
       </c>
       <c r="E32" s="3">
+        <f>D32-1</f>
         <v>1</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H32" s="5">
-        <v>44</v>
+        <v>22.04</v>
       </c>
       <c r="I32" s="5">
-        <v>43.18</v>
+        <v>2.37</v>
       </c>
       <c r="J32" s="5">
-        <v>43.28</v>
+        <v>11.08</v>
       </c>
       <c r="K32" s="5"/>
       <c r="N32" s="6">
-        <f>(D32-1)/$B$32</f>
-        <v>0.25</v>
+        <f t="shared" si="6"/>
+        <v>0.5</v>
       </c>
       <c r="O32" s="6">
-        <f>E32/$B$32</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <f>D33-1</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>16</v>
+      </c>
+      <c r="H33" s="5">
+        <v>22.04</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1.24</v>
+      </c>
+      <c r="J33" s="5">
+        <v>11.07</v>
+      </c>
       <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="10"/>
+      <c r="N33" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="O33" s="6">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="3">
         <v>2</v>
       </c>
       <c r="D34" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="3">
+        <f>D34-1</f>
         <v>1</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="H34" s="5">
-        <v>44</v>
+        <v>22.04</v>
       </c>
       <c r="I34" s="5">
-        <v>21.72</v>
+        <v>0.86</v>
       </c>
       <c r="J34" s="5">
-        <v>21.61</v>
+        <v>11.05</v>
       </c>
       <c r="K34" s="5"/>
       <c r="N34" s="6">
-        <f>(D34-1)/$B$32</f>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="O34" s="6">
-        <f>E34/$B$32</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10"/>
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E35" s="3">
+        <f>D35-1</f>
         <v>1</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="H35" s="5">
-        <v>44</v>
+        <v>22.04</v>
       </c>
       <c r="I35" s="5">
-        <v>10.8</v>
+        <v>0.49</v>
       </c>
       <c r="J35" s="5">
-        <v>10.82</v>
+        <v>11.07</v>
       </c>
       <c r="K35" s="5"/>
       <c r="N35" s="6">
-        <f>(D35-1)/$B$32</f>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.5</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" ref="O35:O45" si="4">E35/$B$32</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="3">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="3">
         <v>5</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D37" s="3">
         <v>9</v>
       </c>
-      <c r="E36" s="3">
-        <v>1</v>
-      </c>
-      <c r="F36" s="3">
-        <f t="shared" si="0"/>
+      <c r="E37" s="3">
+        <f>D37-1</f>
         <v>8</v>
       </c>
-      <c r="H36" s="5">
-        <v>44</v>
-      </c>
-      <c r="I36" s="5">
-        <v>10.83</v>
-      </c>
-      <c r="J36" s="5">
-        <v>5.58</v>
-      </c>
-      <c r="K36" s="5"/>
-      <c r="N36" s="6">
-        <f>(D36-1)/$B$32</f>
-        <v>2</v>
-      </c>
-      <c r="O36" s="6">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="3">
+      <c r="F37" s="3">
+        <v>8</v>
+      </c>
+      <c r="H37" s="5">
+        <v>22.04</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="J37" s="5">
+        <v>1.44</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="3">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3">
         <v>9</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E38" s="3">
+        <f>D38-1</f>
+        <v>8</v>
+      </c>
+      <c r="F38" s="3">
+        <v>16</v>
+      </c>
+      <c r="H38" s="5">
+        <v>22.04</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="J38" s="5">
+        <v>1.44</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="3">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
         <v>17</v>
       </c>
-      <c r="E37" s="3">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3">
-        <f t="shared" si="0"/>
+      <c r="E39" s="3">
+        <f>D39-1</f>
         <v>16</v>
       </c>
-      <c r="H37" s="5">
-        <v>44</v>
-      </c>
-      <c r="I37" s="5">
-        <v>10.58</v>
-      </c>
-      <c r="J37" s="5">
-        <v>2.83</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="N37" s="6">
-        <f>(D37-1)/$B$32</f>
+      <c r="F39" s="3">
+        <v>8</v>
+      </c>
+      <c r="H39" s="5">
+        <v>22.04</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O37" s="6">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="3">
-        <v>17</v>
-      </c>
-      <c r="D38" s="3">
-        <v>33</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="H38" s="5">
-        <v>44</v>
-      </c>
-      <c r="I38" s="5">
-        <v>10.82</v>
-      </c>
-      <c r="J38" s="5">
-        <v>1.57</v>
-      </c>
-      <c r="K38" s="5"/>
-      <c r="N38" s="6">
-        <f>(D38-1)/$B$32</f>
-        <v>8</v>
-      </c>
-      <c r="O38" s="6">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="3">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2</v>
-      </c>
-      <c r="E40" s="3">
-        <v>2</v>
-      </c>
-      <c r="F40" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H40" s="5">
-        <v>44</v>
-      </c>
-      <c r="I40" s="5">
-        <v>21.81</v>
-      </c>
-      <c r="J40" s="5">
-        <v>21.77</v>
-      </c>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="N40" s="6">
-        <f>(D40-1)/$B$32</f>
-        <v>0.25</v>
-      </c>
-      <c r="O40" s="6">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
+      <c r="B41" s="11">
+        <v>4</v>
+      </c>
       <c r="C41" s="3">
         <v>2</v>
       </c>
@@ -2973,584 +2988,571 @@
         <v>2</v>
       </c>
       <c r="E41" s="3">
-        <v>4</v>
+        <f>D41-1</f>
+        <v>1</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H41" s="5">
         <v>44</v>
       </c>
       <c r="I41" s="5">
-        <v>9.48</v>
+        <v>43.18</v>
       </c>
       <c r="J41" s="5">
-        <v>9.58</v>
+        <v>43.28</v>
       </c>
       <c r="K41" s="5"/>
       <c r="N41" s="6">
-        <f>(D41-1)/$B$32</f>
+        <f>(D41-1)/$B$41</f>
         <v>0.25</v>
       </c>
       <c r="O41" s="6">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="3">
-        <v>2</v>
-      </c>
-      <c r="D42" s="3">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3">
-        <v>8</v>
-      </c>
-      <c r="F42" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H42" s="5">
-        <v>44</v>
-      </c>
-      <c r="I42" s="5">
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="J42" s="5">
-        <v>9.7100000000000009</v>
-      </c>
+        <f>F41/$B$41</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="N42" s="6">
-        <f>(D42-1)/$B$32</f>
-        <v>0.25</v>
-      </c>
-      <c r="O42" s="6">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="3">
         <v>2</v>
       </c>
       <c r="D43" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="3">
-        <v>16</v>
+        <f>D43-1</f>
+        <v>2</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H43" s="5">
         <v>44</v>
       </c>
       <c r="I43" s="5">
-        <v>2.39</v>
+        <v>21.72</v>
       </c>
       <c r="J43" s="5">
-        <v>9.68</v>
+        <v>21.61</v>
       </c>
       <c r="K43" s="5"/>
       <c r="N43" s="6">
-        <f>(D43-1)/$B$32</f>
+        <f>(D43-1)/$B$41</f>
+        <v>0.5</v>
+      </c>
+      <c r="O43" s="6">
+        <f>F43/$B$41</f>
         <v>0.25</v>
       </c>
-      <c r="O43" s="6">
-        <f t="shared" si="4"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="12"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5</v>
+      </c>
+      <c r="E44" s="3">
+        <f>D44-1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="3">
-        <v>2</v>
-      </c>
-      <c r="D44" s="3">
-        <v>2</v>
-      </c>
-      <c r="E44" s="3">
-        <v>24</v>
-      </c>
       <c r="F44" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H44" s="5">
         <v>44</v>
       </c>
       <c r="I44" s="5">
-        <v>1.7</v>
+        <v>10.8</v>
       </c>
       <c r="J44" s="5">
-        <v>9.51</v>
+        <v>10.82</v>
       </c>
       <c r="K44" s="5"/>
       <c r="N44" s="6">
-        <f>(D44-1)/$B$32</f>
+        <f>(D44-1)/$B$41</f>
+        <v>1</v>
+      </c>
+      <c r="O44" s="6">
+        <f t="shared" ref="O44:O54" si="7">F44/$B$41</f>
         <v>0.25</v>
       </c>
-      <c r="O44" s="6">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="10"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D45" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E45" s="3">
-        <v>48</v>
+        <f>D45-1</f>
+        <v>8</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H45" s="5">
         <v>44</v>
       </c>
       <c r="I45" s="5">
-        <v>0.95</v>
+        <v>10.83</v>
       </c>
       <c r="J45" s="5">
-        <v>9.68</v>
+        <v>5.58</v>
       </c>
       <c r="K45" s="5"/>
       <c r="N45" s="6">
-        <f>(D45-1)/$B$32</f>
+        <f>(D45-1)/$B$41</f>
+        <v>2</v>
+      </c>
+      <c r="O45" s="6">
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
-      <c r="O45" s="6">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="12"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="3">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3">
+        <v>17</v>
+      </c>
+      <c r="E46" s="3">
+        <f>D46-1</f>
+        <v>16</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>44</v>
+      </c>
+      <c r="I46" s="5">
+        <v>10.58</v>
+      </c>
+      <c r="J46" s="5">
+        <v>2.83</v>
+      </c>
       <c r="K46" s="5"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
-      <c r="B47" s="10">
-        <v>8</v>
-      </c>
+      <c r="N46" s="6">
+        <f>(D46-1)/$B$41</f>
+        <v>4</v>
+      </c>
+      <c r="O46" s="6">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="12"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D47" s="3">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="E47" s="3">
-        <v>1</v>
+        <f>D47-1</f>
+        <v>32</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H47" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I47" s="5">
-        <v>86.87</v>
+        <v>10.82</v>
       </c>
       <c r="J47" s="5">
-        <v>86.71</v>
+        <v>1.57</v>
       </c>
       <c r="K47" s="5"/>
       <c r="N47" s="6">
-        <f>(D47-1)/$B$47</f>
-        <v>0.125</v>
+        <f>(D47-1)/$B$41</f>
+        <v>8</v>
       </c>
       <c r="O47" s="6">
-        <f>E47/$B$47</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
-      <c r="B48" s="10"/>
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" s="12"/>
+      <c r="B48" s="11"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="10"/>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="12"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="3">
         <v>2</v>
       </c>
       <c r="D49" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49" s="3">
+        <f>D49-1</f>
         <v>1</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H49" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I49" s="5">
-        <v>43.87</v>
+        <v>21.81</v>
       </c>
       <c r="J49" s="5">
-        <v>42.21</v>
+        <v>21.77</v>
       </c>
       <c r="K49" s="5"/>
       <c r="N49" s="6">
-        <f>(D49-1)/$B$47</f>
+        <f t="shared" ref="N49:N54" si="8">(D49-1)/$B$41</f>
         <v>0.25</v>
       </c>
       <c r="O49" s="6">
-        <f t="shared" ref="O49:O60" si="5">E49/$B$47</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="11"/>
-      <c r="B50" s="10"/>
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50" s="12"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E50" s="3">
+        <f>D50-1</f>
         <v>1</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H50" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I50" s="5">
-        <v>21.77</v>
+        <v>9.48</v>
       </c>
       <c r="J50" s="5">
-        <v>21.32</v>
+        <v>9.58</v>
       </c>
       <c r="K50" s="5"/>
       <c r="N50" s="6">
-        <f>(D50-1)/$B$47</f>
-        <v>0.5</v>
+        <f t="shared" si="8"/>
+        <v>0.25</v>
       </c>
       <c r="O50" s="6">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="10"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51" s="12"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D51" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E51" s="3">
+        <f>D51-1</f>
         <v>1</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H51" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I51" s="5">
-        <v>11.15</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="J51" s="5">
-        <v>11.16</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="K51" s="5"/>
       <c r="N51" s="6">
-        <f>(D51-1)/$B$47</f>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0.25</v>
       </c>
       <c r="O51" s="6">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="10"/>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52" s="12"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D52" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E52" s="3">
+        <f>D52-1</f>
         <v>1</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H52" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I52" s="5">
-        <v>11.14</v>
+        <v>2.39</v>
       </c>
       <c r="J52" s="5">
-        <v>5.6</v>
+        <v>9.68</v>
       </c>
       <c r="K52" s="5"/>
       <c r="N52" s="6">
-        <f>(D52-1)/$B$47</f>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>0.25</v>
       </c>
       <c r="O52" s="6">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="10"/>
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53" s="12"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D53" s="3">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E53" s="3">
+        <f>D53-1</f>
         <v>1</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H53" s="5">
-        <v>88.02</v>
+        <v>44</v>
       </c>
       <c r="I53" s="5">
-        <v>11.12</v>
+        <v>1.7</v>
       </c>
       <c r="J53" s="5">
-        <v>3</v>
+        <v>9.51</v>
       </c>
       <c r="K53" s="5"/>
       <c r="N53" s="6">
-        <f>(D53-1)/$B$47</f>
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O53" s="6">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="3">
+        <v>2</v>
+      </c>
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="3">
+        <f>D54-1</f>
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>48</v>
+      </c>
+      <c r="H54" s="5">
+        <v>44</v>
+      </c>
+      <c r="I54" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="J54" s="5">
+        <v>9.68</v>
+      </c>
+      <c r="K54" s="5"/>
+      <c r="N54" s="6">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O54" s="6">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="12"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="3">
+        <v>5</v>
+      </c>
+      <c r="D56" s="3">
+        <v>9</v>
+      </c>
+      <c r="E56" s="3">
+        <f>D56-1</f>
+        <v>8</v>
+      </c>
+      <c r="F56" s="3">
+        <v>8</v>
+      </c>
+      <c r="H56" s="5">
+        <v>44</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1.24</v>
+      </c>
+      <c r="J56" s="5">
+        <v>1.31</v>
+      </c>
+      <c r="K56" s="5"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10">
+        <f>(D56-1)/$B$41</f>
+        <v>2</v>
+      </c>
+      <c r="O56" s="10">
+        <f>F56/$B$41</f>
+        <v>2</v>
+      </c>
+      <c r="P56" s="10"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="12"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="3">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3">
+        <v>9</v>
+      </c>
+      <c r="E57" s="3">
+        <f>D57-1</f>
+        <v>8</v>
+      </c>
+      <c r="F57" s="3">
+        <v>16</v>
+      </c>
+      <c r="H57" s="5">
+        <v>44</v>
+      </c>
+      <c r="I57" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="J57" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="K57" s="5"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10">
+        <f>(D57-1)/$B$41</f>
+        <v>2</v>
+      </c>
+      <c r="O57" s="10">
+        <f>F57/$B$41</f>
         <v>4</v>
       </c>
-      <c r="O53" s="6">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
-      <c r="B54" s="10"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A55" s="11"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="3">
-        <v>2</v>
-      </c>
-      <c r="D55" s="3">
-        <v>2</v>
-      </c>
-      <c r="E55" s="3">
-        <v>2</v>
-      </c>
-      <c r="F55" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H55" s="5">
-        <v>88.02</v>
-      </c>
-      <c r="I55" s="5">
-        <v>41.6</v>
-      </c>
-      <c r="J55" s="5">
-        <v>41.76</v>
-      </c>
-      <c r="K55" s="5"/>
-      <c r="N55" s="6">
-        <f>(D55-1)/$B$47</f>
-        <v>0.125</v>
-      </c>
-      <c r="O55" s="6">
-        <f t="shared" si="5"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="3">
-        <v>2</v>
-      </c>
-      <c r="D56" s="3">
-        <v>2</v>
-      </c>
-      <c r="E56" s="3">
+      <c r="P57" s="10"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="3">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3">
+        <v>17</v>
+      </c>
+      <c r="E58" s="3">
+        <f>D58-1</f>
+        <v>16</v>
+      </c>
+      <c r="F58" s="3">
+        <v>8</v>
+      </c>
+      <c r="H58" s="5">
+        <v>44</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1.24</v>
+      </c>
+      <c r="J58" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="K58" s="5"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10">
+        <f>(D58-1)/$B$41</f>
         <v>4</v>
       </c>
-      <c r="F56" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H56" s="5">
-        <v>88.02</v>
-      </c>
-      <c r="I56" s="5">
-        <v>18.989999999999998</v>
-      </c>
-      <c r="J56" s="5">
-        <v>19.05</v>
-      </c>
-      <c r="K56" s="5"/>
-      <c r="N56" s="6">
-        <f>(D56-1)/$B$47</f>
-        <v>0.125</v>
-      </c>
-      <c r="O56" s="6">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="3">
-        <v>2</v>
-      </c>
-      <c r="D57" s="3">
-        <v>2</v>
-      </c>
-      <c r="E57" s="3">
+      <c r="O58" s="10">
+        <f>F58/$B$41</f>
+        <v>2</v>
+      </c>
+      <c r="P58" s="10"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59" s="12"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60" s="12"/>
+      <c r="B60" s="11">
         <v>8</v>
       </c>
-      <c r="F57" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H57" s="5">
-        <v>88.02</v>
-      </c>
-      <c r="I57" s="5">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="J57" s="5">
-        <v>9.52</v>
-      </c>
-      <c r="K57" s="5"/>
-      <c r="N57" s="6">
-        <f>(D57-1)/$B$47</f>
-        <v>0.125</v>
-      </c>
-      <c r="O57" s="6">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="3">
-        <v>2</v>
-      </c>
-      <c r="D58" s="3">
-        <v>2</v>
-      </c>
-      <c r="E58" s="3">
-        <v>16</v>
-      </c>
-      <c r="F58" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H58" s="5">
-        <v>88.02</v>
-      </c>
-      <c r="I58" s="5">
-        <v>4.82</v>
-      </c>
-      <c r="J58" s="5">
-        <v>9.39</v>
-      </c>
-      <c r="K58" s="5"/>
-      <c r="N58" s="6">
-        <f>(D58-1)/$B$47</f>
-        <v>0.125</v>
-      </c>
-      <c r="O58" s="6">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="11"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="3">
-        <v>2</v>
-      </c>
-      <c r="D59" s="3">
-        <v>2</v>
-      </c>
-      <c r="E59" s="3">
-        <v>24</v>
-      </c>
-      <c r="F59" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H59" s="5">
-        <v>88.02</v>
-      </c>
-      <c r="I59" s="5">
-        <v>3.37</v>
-      </c>
-      <c r="J59" s="5">
-        <v>9.52</v>
-      </c>
-      <c r="K59" s="5"/>
-      <c r="N59" s="6">
-        <f>(D59-1)/$B$47</f>
-        <v>0.125</v>
-      </c>
-      <c r="O59" s="6">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="11"/>
-      <c r="B60" s="10"/>
       <c r="C60" s="3">
         <v>2</v>
       </c>
@@ -3558,87 +3560,1187 @@
         <v>2</v>
       </c>
       <c r="E60" s="3">
-        <v>48</v>
+        <f>D60-1</f>
+        <v>1</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H60" s="5">
         <v>88.02</v>
       </c>
       <c r="I60" s="5">
-        <v>1.87</v>
+        <v>86.87</v>
       </c>
       <c r="J60" s="5">
-        <v>9.3800000000000008</v>
+        <v>86.71</v>
       </c>
       <c r="K60" s="5"/>
       <c r="N60" s="6">
-        <f>(D60-1)/$B$47</f>
+        <f>(D60-1)/$B$60</f>
         <v>0.125</v>
       </c>
       <c r="O60" s="6">
-        <f t="shared" si="5"/>
+        <f>F60/$B$60</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="12"/>
+      <c r="B61" s="11"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="12"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="3">
+        <v>2</v>
+      </c>
+      <c r="D62" s="3">
+        <v>3</v>
+      </c>
+      <c r="E62" s="3">
+        <f>D62-1</f>
+        <v>2</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="H62" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I62" s="5">
+        <v>43.87</v>
+      </c>
+      <c r="J62" s="5">
+        <v>42.21</v>
+      </c>
+      <c r="K62" s="5"/>
+      <c r="N62" s="6">
+        <f>(D62-1)/$B$60</f>
+        <v>0.25</v>
+      </c>
+      <c r="O62" s="6">
+        <f t="shared" ref="O62:O72" si="9">F62/$B$60</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="12"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="3">
+        <v>3</v>
+      </c>
+      <c r="D63" s="3">
+        <v>5</v>
+      </c>
+      <c r="E63" s="3">
+        <f>D63-1</f>
+        <v>4</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="H63" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I63" s="5">
+        <v>21.77</v>
+      </c>
+      <c r="J63" s="5">
+        <v>21.32</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="N63" s="6">
+        <f>(D63-1)/$B$60</f>
+        <v>0.5</v>
+      </c>
+      <c r="O63" s="6">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="3">
+        <v>5</v>
+      </c>
+      <c r="D64" s="3">
+        <v>9</v>
+      </c>
+      <c r="E64" s="3">
+        <f>D64-1</f>
+        <v>8</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="H64" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I64" s="5">
+        <v>11.15</v>
+      </c>
+      <c r="J64" s="5">
+        <v>11.16</v>
+      </c>
+      <c r="K64" s="5"/>
+      <c r="N64" s="6">
+        <f>(D64-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O64" s="6">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A65" s="12"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="3">
+        <v>9</v>
+      </c>
+      <c r="D65" s="3">
+        <v>17</v>
+      </c>
+      <c r="E65" s="3">
+        <f>D65-1</f>
+        <v>16</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="H65" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I65" s="5">
+        <v>11.14</v>
+      </c>
+      <c r="J65" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="K65" s="5"/>
+      <c r="N65" s="6">
+        <f>(D65-1)/$B$60</f>
+        <v>2</v>
+      </c>
+      <c r="O65" s="6">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="3">
+        <v>17</v>
+      </c>
+      <c r="D66" s="3">
+        <v>33</v>
+      </c>
+      <c r="E66" s="3">
+        <f>D66-1</f>
+        <v>32</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
+      <c r="H66" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I66" s="5">
+        <v>11.12</v>
+      </c>
+      <c r="J66" s="5">
+        <v>3</v>
+      </c>
+      <c r="K66" s="5"/>
+      <c r="N66" s="6">
+        <f>(D66-1)/$B$60</f>
+        <v>4</v>
+      </c>
+      <c r="O66" s="6">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A67" s="12"/>
+      <c r="B67" s="11"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A68" s="12"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="3">
+        <v>2</v>
+      </c>
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="3">
+        <f>D68-1</f>
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>2</v>
+      </c>
+      <c r="H68" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I68" s="5">
+        <v>41.6</v>
+      </c>
+      <c r="J68" s="5">
+        <v>41.76</v>
+      </c>
+      <c r="K68" s="5"/>
+      <c r="N68" s="6">
+        <f t="shared" ref="N68:N72" si="10">(D68-1)/$B$60</f>
+        <v>0.125</v>
+      </c>
+      <c r="O68" s="6">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="3">
+        <v>2</v>
+      </c>
+      <c r="D69" s="3">
+        <v>2</v>
+      </c>
+      <c r="E69" s="3">
+        <f>D69-1</f>
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
+        <v>4</v>
+      </c>
+      <c r="H69" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I69" s="5">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="J69" s="5">
+        <v>19.05</v>
+      </c>
+      <c r="K69" s="5"/>
+      <c r="N69" s="6">
+        <f t="shared" si="10"/>
+        <v>0.125</v>
+      </c>
+      <c r="O69" s="6">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A70" s="12"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="3">
+        <v>2</v>
+      </c>
+      <c r="D70" s="3">
+        <v>2</v>
+      </c>
+      <c r="E70" s="3">
+        <f>D70-1</f>
+        <v>1</v>
+      </c>
+      <c r="F70" s="3">
+        <v>8</v>
+      </c>
+      <c r="H70" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I70" s="5">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="J70" s="5">
+        <v>9.52</v>
+      </c>
+      <c r="K70" s="5"/>
+      <c r="N70" s="6">
+        <f t="shared" si="10"/>
+        <v>0.125</v>
+      </c>
+      <c r="O70" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="3">
+        <v>2</v>
+      </c>
+      <c r="D71" s="3">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3">
+        <f>D71-1</f>
+        <v>1</v>
+      </c>
+      <c r="F71" s="3">
+        <v>16</v>
+      </c>
+      <c r="H71" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I71" s="5">
+        <v>4.82</v>
+      </c>
+      <c r="J71" s="5">
+        <v>9.39</v>
+      </c>
+      <c r="K71" s="5"/>
+      <c r="N71" s="6">
+        <f t="shared" si="10"/>
+        <v>0.125</v>
+      </c>
+      <c r="O71" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A72" s="12"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="3">
+        <v>2</v>
+      </c>
+      <c r="D72" s="3">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3">
+        <f>D72-1</f>
+        <v>1</v>
+      </c>
+      <c r="F72" s="3">
+        <v>24</v>
+      </c>
+      <c r="H72" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I72" s="5">
+        <v>3.37</v>
+      </c>
+      <c r="J72" s="5">
+        <v>9.52</v>
+      </c>
+      <c r="K72" s="5"/>
+      <c r="N72" s="6">
+        <f t="shared" si="10"/>
+        <v>0.125</v>
+      </c>
+      <c r="O72" s="6">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A73" s="12"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="3">
+        <v>2</v>
+      </c>
+      <c r="D73" s="3">
+        <v>2</v>
+      </c>
+      <c r="E73" s="3">
+        <f>D73-1</f>
+        <v>1</v>
+      </c>
+      <c r="F73" s="3">
+        <v>48</v>
+      </c>
+      <c r="H73" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I73" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="J73" s="5">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="K73" s="5"/>
+      <c r="N73" s="6">
+        <f>(D73-1)/$B$60</f>
+        <v>0.125</v>
+      </c>
+      <c r="O73" s="6">
+        <f>F73/$B$60</f>
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="11" t="s">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A74" s="12"/>
+      <c r="B74" s="11"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A75" s="12"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="3">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3">
+        <v>9</v>
+      </c>
+      <c r="E75" s="3">
+        <f>D75-1</f>
+        <v>8</v>
+      </c>
+      <c r="F75" s="3">
+        <v>8</v>
+      </c>
+      <c r="H75" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I75" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="J75" s="5">
+        <v>1.27</v>
+      </c>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="10">
+        <f t="shared" ref="N75:N77" si="11">(D75-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O75" s="10">
+        <f t="shared" ref="O75:O77" si="12">F75/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="6"/>
+      <c r="U75" s="6"/>
+      <c r="V75" s="6"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="6"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="3">
+        <v>5</v>
+      </c>
+      <c r="D76" s="3">
+        <v>9</v>
+      </c>
+      <c r="E76" s="3">
+        <f>D76-1</f>
+        <v>8</v>
+      </c>
+      <c r="F76" s="3">
+        <v>16</v>
+      </c>
+      <c r="H76" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I76" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="J76" s="5">
+        <v>1.28</v>
+      </c>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="10">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O76" s="10">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="6"/>
+      <c r="U76" s="6"/>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="6"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A77" s="12"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="3">
+        <v>9</v>
+      </c>
+      <c r="D77" s="3">
+        <v>17</v>
+      </c>
+      <c r="E77" s="3">
+        <f>D77-1</f>
+        <v>16</v>
+      </c>
+      <c r="F77" s="3">
+        <v>8</v>
+      </c>
+      <c r="H77" s="5">
+        <v>88.02</v>
+      </c>
+      <c r="I77" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="J77" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="10">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="O77" s="10">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="6"/>
+      <c r="U77" s="6"/>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A78" s="13"/>
+      <c r="B78" s="7"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A79" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B79" s="11">
+        <v>3</v>
+      </c>
+      <c r="C79" s="3">
+        <v>2</v>
+      </c>
+      <c r="D79" s="3">
+        <v>3</v>
+      </c>
+      <c r="E79" s="3">
+        <f>D79-1</f>
+        <v>2</v>
+      </c>
+      <c r="F79" s="3">
+        <v>2</v>
+      </c>
+      <c r="I79" s="14">
+        <v>86.01</v>
+      </c>
+      <c r="J79" s="5">
+        <v>97.1</v>
+      </c>
+      <c r="N79" s="10">
+        <f>(D79-1)/$B$60</f>
+        <v>0.25</v>
+      </c>
+      <c r="O79" s="10">
+        <f>F79/$B$60</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A80" s="12"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="3">
+        <v>5</v>
+      </c>
+      <c r="D80" s="3">
+        <v>9</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" ref="E80:E98" si="13">D80-1</f>
+        <v>8</v>
+      </c>
+      <c r="F80" s="3">
+        <v>8</v>
+      </c>
+      <c r="I80" s="14">
+        <v>10.36</v>
+      </c>
+      <c r="J80" s="14">
+        <v>10.7</v>
+      </c>
+      <c r="N80" s="10">
+        <f>(D80-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O80" s="10">
+        <f>F80/$B$60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A81" s="12"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="3">
+        <v>5</v>
+      </c>
+      <c r="D81" s="3">
+        <v>9</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F81" s="3">
+        <v>10</v>
+      </c>
+      <c r="I81" s="14">
+        <v>8.34</v>
+      </c>
+      <c r="J81" s="14">
+        <v>10.67</v>
+      </c>
+      <c r="N81" s="10">
+        <f>(D81-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O81" s="10">
+        <f>F81/$B$60</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A82" s="12"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="3">
+        <v>5</v>
+      </c>
+      <c r="D82" s="3">
+        <v>9</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F82" s="3">
+        <v>16</v>
+      </c>
+      <c r="H82" s="5"/>
+      <c r="I82" s="14">
+        <v>5.37</v>
+      </c>
+      <c r="J82" s="14">
+        <v>10.78</v>
+      </c>
+      <c r="N82" s="10">
+        <f>(D82-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O82" s="10">
+        <f>F82/$B$60</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A83" s="12"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="3">
+        <v>9</v>
+      </c>
+      <c r="D83" s="3">
+        <v>17</v>
+      </c>
+      <c r="E83" s="3">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="F83" s="3">
+        <v>8</v>
+      </c>
+      <c r="H83" s="5"/>
+      <c r="I83" s="14">
+        <v>10.3</v>
+      </c>
+      <c r="J83" s="14">
+        <v>5.48</v>
+      </c>
+      <c r="N83" s="10">
+        <f>(D83-1)/$B$60</f>
+        <v>2</v>
+      </c>
+      <c r="O83" s="10">
+        <f>F83/$B$60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A84" s="12"/>
+      <c r="B84" s="10"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A85" s="12"/>
+      <c r="B85" s="11">
         <v>4</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="11"/>
-      <c r="B63" s="10"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A64" s="11"/>
-      <c r="B64" s="10"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="11"/>
-      <c r="B65" s="10"/>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="11"/>
-      <c r="B66" s="10"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="11"/>
-      <c r="B67" s="10"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="11"/>
-      <c r="B68" s="10"/>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="10"/>
-      <c r="H69" s="5"/>
+      <c r="C85" s="3">
+        <v>3</v>
+      </c>
+      <c r="D85" s="3">
+        <v>5</v>
+      </c>
+      <c r="E85" s="3">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="I85" s="14">
+        <v>96.44</v>
+      </c>
+      <c r="J85" s="14">
+        <v>96.67</v>
+      </c>
+      <c r="N85" s="10">
+        <f>(D85-1)/$B$60</f>
+        <v>0.5</v>
+      </c>
+      <c r="O85" s="10">
+        <f>F85/$B$60</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A86" s="12"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="3">
+        <v>17</v>
+      </c>
+      <c r="D86" s="3">
+        <v>33</v>
+      </c>
+      <c r="E86" s="3">
+        <f t="shared" si="13"/>
+        <v>32</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="I86" s="14">
+        <v>96.35</v>
+      </c>
+      <c r="J86" s="14">
+        <v>12.5</v>
+      </c>
+      <c r="N86" s="10">
+        <f>(D86-1)/$B$60</f>
+        <v>4</v>
+      </c>
+      <c r="O86" s="10">
+        <f>F86/$B$60</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A87" s="12"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="3">
+        <v>5</v>
+      </c>
+      <c r="D87" s="3">
+        <v>9</v>
+      </c>
+      <c r="E87" s="3">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F87" s="3">
+        <v>2</v>
+      </c>
+      <c r="I87" s="4">
+        <v>48.72</v>
+      </c>
+      <c r="J87" s="4">
+        <v>24.67</v>
+      </c>
+      <c r="N87" s="10">
+        <f>(D87-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O87" s="10">
+        <f>F87/$B$60</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A88" s="12"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="3">
+        <v>5</v>
+      </c>
+      <c r="D88" s="3">
+        <v>9</v>
+      </c>
+      <c r="E88" s="3">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F88" s="3">
+        <v>8</v>
+      </c>
+      <c r="I88" s="14">
+        <v>10.33</v>
+      </c>
+      <c r="J88" s="14">
+        <v>10.77</v>
+      </c>
+      <c r="N88" s="10">
+        <f>(D88-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O88" s="10">
+        <f>F88/$B$60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A89" s="12"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="3">
+        <v>5</v>
+      </c>
+      <c r="D89" s="3">
+        <v>9</v>
+      </c>
+      <c r="E89" s="3">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F89" s="3">
+        <v>16</v>
+      </c>
+      <c r="I89" s="14">
+        <v>5.34</v>
+      </c>
+      <c r="J89" s="14">
+        <v>10.67</v>
+      </c>
+      <c r="N89" s="10">
+        <f>(D89-1)/$B$60</f>
+        <v>1</v>
+      </c>
+      <c r="O89" s="10">
+        <f>F89/$B$60</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A90" s="12"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="3">
+        <v>9</v>
+      </c>
+      <c r="D90" s="3">
+        <v>17</v>
+      </c>
+      <c r="E90" s="3">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="F90" s="3">
+        <v>8</v>
+      </c>
+      <c r="I90" s="14">
+        <v>10.41</v>
+      </c>
+      <c r="J90" s="14">
+        <v>5.44</v>
+      </c>
+      <c r="N90" s="10">
+        <f>(D90-1)/$B$60</f>
+        <v>2</v>
+      </c>
+      <c r="O90" s="10">
+        <f>F90/$B$60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A91" s="12"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="3">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <v>2</v>
+      </c>
+      <c r="E91" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>4</v>
+      </c>
+      <c r="I91" s="14">
+        <v>83.16</v>
+      </c>
+      <c r="J91" s="14">
+        <v>83.07</v>
+      </c>
+      <c r="N91" s="10">
+        <f>(D91-1)/$B$60</f>
+        <v>0.125</v>
+      </c>
+      <c r="O91" s="10">
+        <f>F91/$B$60</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A92" s="12"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="3">
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <v>2</v>
+      </c>
+      <c r="E92" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="F92" s="3">
+        <v>48</v>
+      </c>
+      <c r="I92" s="14">
+        <v>8.15</v>
+      </c>
+      <c r="J92" s="14">
+        <v>81.78</v>
+      </c>
+      <c r="N92" s="10"/>
+      <c r="O92" s="10"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A93" s="12"/>
+      <c r="B93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A94" s="12"/>
+      <c r="B94" s="11">
+        <v>6</v>
+      </c>
+      <c r="C94" s="3">
+        <v>3</v>
+      </c>
+      <c r="D94" s="3">
+        <v>5</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="F94" s="3">
+        <v>3</v>
+      </c>
+      <c r="I94" s="14">
+        <v>57.22</v>
+      </c>
+      <c r="J94" s="14">
+        <v>42.42</v>
+      </c>
+      <c r="N94" s="10">
+        <f t="shared" ref="N94:N98" si="14">(D94-1)/$B$60</f>
+        <v>0.5</v>
+      </c>
+      <c r="O94" s="10">
+        <f t="shared" ref="O94:O98" si="15">F94/$B$60</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A95" s="12"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="3">
+        <v>3</v>
+      </c>
+      <c r="D95" s="3">
+        <v>5</v>
+      </c>
+      <c r="E95" s="3">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="F95" s="3">
+        <v>5</v>
+      </c>
+      <c r="I95" s="14">
+        <v>31.3</v>
+      </c>
+      <c r="J95" s="14">
+        <v>20.25</v>
+      </c>
+      <c r="N95" s="10">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O95" s="10">
+        <f t="shared" si="15"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A96" s="12"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="3">
+        <v>3</v>
+      </c>
+      <c r="D96" s="3">
+        <v>5</v>
+      </c>
+      <c r="E96" s="3">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="F96" s="3">
+        <v>8</v>
+      </c>
+      <c r="I96" s="14">
+        <v>20.25</v>
+      </c>
+      <c r="J96" s="14">
+        <v>20.49</v>
+      </c>
+      <c r="N96" s="10">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="O96" s="10">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="3">
+        <v>5</v>
+      </c>
+      <c r="D97" s="3">
+        <v>10</v>
+      </c>
+      <c r="E97" s="3">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="F97" s="3">
+        <v>5</v>
+      </c>
+      <c r="I97" s="14">
+        <v>16.3</v>
+      </c>
+      <c r="J97" s="14">
+        <v>19.7</v>
+      </c>
+      <c r="N97" s="10">
+        <f t="shared" si="14"/>
+        <v>1.125</v>
+      </c>
+      <c r="O97" s="10">
+        <f t="shared" si="15"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="3">
+        <v>6</v>
+      </c>
+      <c r="D98" s="3">
+        <v>12</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="13"/>
+        <v>11</v>
+      </c>
+      <c r="F98" s="3">
+        <v>5</v>
+      </c>
+      <c r="I98" s="14">
+        <v>16.2</v>
+      </c>
+      <c r="J98" s="14">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="N98" s="10">
+        <f t="shared" si="14"/>
+        <v>1.375</v>
+      </c>
+      <c r="O98" s="10">
+        <f t="shared" si="15"/>
+        <v>0.625</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B62:B69"/>
-    <mergeCell ref="A62:A69"/>
-    <mergeCell ref="B2:B15"/>
-    <mergeCell ref="B17:B30"/>
-    <mergeCell ref="B32:B45"/>
-    <mergeCell ref="B47:B60"/>
-    <mergeCell ref="A2:A60"/>
+  <mergeCells count="9">
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B85:B92"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="A79:A98"/>
+    <mergeCell ref="B41:B58"/>
+    <mergeCell ref="B60:B77"/>
+    <mergeCell ref="A2:A77"/>
+    <mergeCell ref="B22:B39"/>
+    <mergeCell ref="B2:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add results of gpu experiments
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A86FA4E-8FDB-423F-9180-BA0EAEF70050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBC12C-2E6C-4454-9AC7-8E0B5268DACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hybrid - No GPU" sheetId="1" r:id="rId1"/>
+    <sheet name="With GPU" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t># Nodes</t>
   </si>
@@ -102,6 +103,24 @@
   <si>
     <t># Active Ranks</t>
   </si>
+  <si>
+    <t>Patterns Over Ranks - GPU taking 50% of job  [s]</t>
+  </si>
+  <si>
+    <t>Patterns Over Ranks - GPU taking 75% of job [s]</t>
+  </si>
+  <si>
+    <t>Patterns Over Ranks - No GPU [s]</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Levenshtein Computation Executed</t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +193,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1591,9 +1622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5605-5B40-4E95-A326-20DE76CB0444}">
   <dimension ref="A1:X98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1662,10 +1693,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="15">
         <v>1</v>
       </c>
       <c r="C2" s="3">
@@ -1713,16 +1744,16 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="15"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1774,8 +1805,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="3">
         <v>3</v>
       </c>
@@ -1821,8 +1852,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1868,8 +1899,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="3">
         <v>9</v>
       </c>
@@ -1918,8 +1949,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3">
         <v>17</v>
       </c>
@@ -1968,16 +1999,16 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="15"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="3">
         <v>2</v>
       </c>
@@ -1985,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="3">
-        <f>D10-1</f>
+        <f t="shared" ref="E10:E15" si="0">D10-1</f>
         <v>1</v>
       </c>
       <c r="F10" s="3">
@@ -2002,29 +2033,29 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="6">
-        <f t="shared" ref="L10:L15" si="0">((D10-1)-1)*F10</f>
+        <f t="shared" ref="L10:L15" si="1">((D10-1)-1)*F10</f>
         <v>0</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" ref="M10:M15" si="1">(D10-1)*(F10-1)</f>
+        <f t="shared" ref="M10:M15" si="2">(D10-1)*(F10-1)</f>
         <v>1</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" ref="N10:N19" si="2">(D10-1)/$B$2</f>
+        <f t="shared" ref="N10:N19" si="3">(D10-1)/$B$2</f>
         <v>1</v>
       </c>
       <c r="O10" s="6">
-        <f>F10/$B$2</f>
+        <f t="shared" ref="O10:O15" si="4">F10/$B$2</f>
         <v>2</v>
       </c>
       <c r="P10" s="6" t="str">
-        <f t="shared" ref="P10:P15" si="3">IF(L10&lt;M10, "Lino", "Paolo")</f>
+        <f t="shared" ref="P10:P15" si="5">IF(L10&lt;M10, "Lino", "Paolo")</f>
         <v>Lino</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -2032,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
-        <f>D11-1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F11" s="3">
@@ -2049,37 +2080,37 @@
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>Lino</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N11" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O11" s="6">
-        <f>F11/$B$2</f>
-        <v>4</v>
-      </c>
-      <c r="P11" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>Lino</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="3">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3">
-        <f>D12-1</f>
         <v>1</v>
       </c>
       <c r="F12" s="3">
@@ -2096,37 +2127,37 @@
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="P12" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>Lino</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="6">
-        <f>F12/$B$2</f>
-        <v>8</v>
-      </c>
-      <c r="P12" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>Lino</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3">
-        <f>D13-1</f>
         <v>1</v>
       </c>
       <c r="F13" s="3">
@@ -2143,37 +2174,37 @@
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="P13" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>Lino</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="N13" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="6">
-        <f>F13/$B$2</f>
-        <v>16</v>
-      </c>
-      <c r="P13" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>Lino</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="3">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3">
-        <f>D14-1</f>
         <v>1</v>
       </c>
       <c r="F14" s="3">
@@ -2190,37 +2221,37 @@
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="P14" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>Lino</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="N14" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="6">
-        <f>F14/$B$2</f>
-        <v>24</v>
-      </c>
-      <c r="P14" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>Lino</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3">
-        <f>D15-1</f>
         <v>1</v>
       </c>
       <c r="F15" s="3">
@@ -2237,29 +2268,29 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O15" s="6">
-        <f>F15/$B$2</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="P15" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Lino</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2271,8 +2302,8 @@
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="3">
         <v>5</v>
       </c>
@@ -2299,18 +2330,18 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" ref="O17:O19" si="4">F17/$B$2</f>
+        <f t="shared" ref="O17:O19" si="6">F17/$B$2</f>
         <v>8</v>
       </c>
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="3">
         <v>5</v>
       </c>
@@ -2337,18 +2368,18 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3">
         <v>9</v>
       </c>
@@ -2375,17 +2406,17 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="10"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2398,15 +2429,15 @@
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+      <c r="A21" s="16"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="11">
+      <c r="A22" s="16"/>
+      <c r="B22" s="15">
         <v>2</v>
       </c>
       <c r="C22" s="3">
@@ -2442,16 +2473,16 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="15"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3">
         <v>2</v>
       </c>
@@ -2485,8 +2516,8 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="3">
         <v>3</v>
       </c>
@@ -2515,13 +2546,13 @@
         <v>2</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" ref="O25:O39" si="5">F25/$B$22</f>
+        <f t="shared" ref="O25:O39" si="7">F25/$B$22</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="3">
         <v>5</v>
       </c>
@@ -2550,13 +2581,13 @@
         <v>4</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="3">
         <v>9</v>
       </c>
@@ -2585,13 +2616,13 @@
         <v>8</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3">
         <v>17</v>
       </c>
@@ -2620,21 +2651,21 @@
         <v>16</v>
       </c>
       <c r="O28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="15"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="11"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3">
         <v>2</v>
       </c>
@@ -2642,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="3">
-        <f>D30-1</f>
+        <f t="shared" ref="E30:E35" si="8">D30-1</f>
         <v>1</v>
       </c>
       <c r="F30" s="3">
@@ -2659,17 +2690,17 @@
       </c>
       <c r="K30" s="5"/>
       <c r="N30" s="6">
-        <f t="shared" ref="N30:N39" si="6">(D30-1)/$B$22</f>
+        <f t="shared" ref="N30:N39" si="9">(D30-1)/$B$22</f>
         <v>0.5</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3">
         <v>2</v>
       </c>
@@ -2677,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="3">
-        <f>D31-1</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F31" s="3">
@@ -2694,17 +2725,17 @@
       </c>
       <c r="K31" s="5"/>
       <c r="N31" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3">
         <v>2</v>
       </c>
@@ -2712,7 +2743,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="3">
-        <f>D32-1</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F32" s="3">
@@ -2729,17 +2760,17 @@
       </c>
       <c r="K32" s="5"/>
       <c r="N32" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="O32" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="3">
         <v>2</v>
       </c>
@@ -2747,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="3">
-        <f>D33-1</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F33" s="3">
@@ -2764,17 +2795,17 @@
       </c>
       <c r="K33" s="5"/>
       <c r="N33" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="3">
         <v>2</v>
       </c>
@@ -2782,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="3">
-        <f>D34-1</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F34" s="3">
@@ -2799,17 +2830,17 @@
       </c>
       <c r="K34" s="5"/>
       <c r="N34" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="3">
         <v>2</v>
       </c>
@@ -2817,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="3">
-        <f>D35-1</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F35" s="3">
@@ -2834,17 +2865,17 @@
       </c>
       <c r="K35" s="5"/>
       <c r="N35" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="15"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -2856,8 +2887,8 @@
       <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="3">
         <v>5</v>
       </c>
@@ -2884,18 +2915,18 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="P37" s="10"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="3">
         <v>5</v>
       </c>
@@ -2922,18 +2953,18 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O38" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="P38" s="10"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="3">
         <v>9</v>
       </c>
@@ -2960,25 +2991,25 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="O39" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="P39" s="10"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="11">
+      <c r="A41" s="16"/>
+      <c r="B41" s="15">
         <v>4</v>
       </c>
       <c r="C41" s="3">
@@ -3014,16 +3045,16 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="15"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="3">
         <v>2</v>
       </c>
@@ -3057,8 +3088,8 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="3">
         <v>3</v>
       </c>
@@ -3087,13 +3118,13 @@
         <v>1</v>
       </c>
       <c r="O44" s="6">
-        <f t="shared" ref="O44:O54" si="7">F44/$B$41</f>
+        <f t="shared" ref="O44:O54" si="10">F44/$B$41</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="11"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="3">
         <v>5</v>
       </c>
@@ -3122,13 +3153,13 @@
         <v>2</v>
       </c>
       <c r="O45" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="11"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="3">
         <v>9</v>
       </c>
@@ -3157,13 +3188,13 @@
         <v>4</v>
       </c>
       <c r="O46" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="3">
         <v>17</v>
       </c>
@@ -3192,21 +3223,21 @@
         <v>8</v>
       </c>
       <c r="O47" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="15"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="11"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="3">
         <v>2</v>
       </c>
@@ -3214,7 +3245,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="3">
-        <f>D49-1</f>
+        <f t="shared" ref="E49:E54" si="11">D49-1</f>
         <v>1</v>
       </c>
       <c r="F49" s="3">
@@ -3231,17 +3262,17 @@
       </c>
       <c r="K49" s="5"/>
       <c r="N49" s="6">
-        <f t="shared" ref="N49:N54" si="8">(D49-1)/$B$41</f>
+        <f t="shared" ref="N49:N54" si="12">(D49-1)/$B$41</f>
         <v>0.25</v>
       </c>
       <c r="O49" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="11"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="3">
         <v>2</v>
       </c>
@@ -3249,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="3">
-        <f>D50-1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F50" s="3">
@@ -3266,17 +3297,17 @@
       </c>
       <c r="K50" s="5"/>
       <c r="N50" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="O50" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="11"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="3">
         <v>2</v>
       </c>
@@ -3284,7 +3315,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="3">
-        <f>D51-1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F51" s="3">
@@ -3301,17 +3332,17 @@
       </c>
       <c r="K51" s="5"/>
       <c r="N51" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="O51" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A52" s="12"/>
-      <c r="B52" s="11"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="3">
         <v>2</v>
       </c>
@@ -3319,7 +3350,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="3">
-        <f>D52-1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F52" s="3">
@@ -3336,17 +3367,17 @@
       </c>
       <c r="K52" s="5"/>
       <c r="N52" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="O52" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="11"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="3">
         <v>2</v>
       </c>
@@ -3354,7 +3385,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="3">
-        <f>D53-1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F53" s="3">
@@ -3371,17 +3402,17 @@
       </c>
       <c r="K53" s="5"/>
       <c r="N53" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="O53" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="11"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="3">
         <v>2</v>
       </c>
@@ -3389,7 +3420,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="3">
-        <f>D54-1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F54" s="3">
@@ -3406,17 +3437,17 @@
       </c>
       <c r="K54" s="5"/>
       <c r="N54" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="O54" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="15"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -3428,8 +3459,8 @@
       <c r="P55" s="10"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="11"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="3">
         <v>5</v>
       </c>
@@ -3466,8 +3497,8 @@
       <c r="P56" s="10"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="11"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="3">
         <v>5</v>
       </c>
@@ -3504,8 +3535,8 @@
       <c r="P57" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="11"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="3">
         <v>9</v>
       </c>
@@ -3542,15 +3573,15 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
+      <c r="A59" s="16"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
-      <c r="B60" s="11">
+      <c r="A60" s="16"/>
+      <c r="B60" s="15">
         <v>8</v>
       </c>
       <c r="C60" s="3">
@@ -3586,16 +3617,16 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="11"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="15"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="12"/>
-      <c r="B62" s="11"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="3">
         <v>2</v>
       </c>
@@ -3624,13 +3655,13 @@
         <v>0.25</v>
       </c>
       <c r="O62" s="6">
-        <f t="shared" ref="O62:O72" si="9">F62/$B$60</f>
+        <f t="shared" ref="O62:O72" si="13">F62/$B$60</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="11"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="15"/>
       <c r="C63" s="3">
         <v>3</v>
       </c>
@@ -3659,13 +3690,13 @@
         <v>0.5</v>
       </c>
       <c r="O63" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-      <c r="B64" s="11"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="3">
         <v>5</v>
       </c>
@@ -3694,13 +3725,13 @@
         <v>1</v>
       </c>
       <c r="O64" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="11"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="3">
         <v>9</v>
       </c>
@@ -3729,13 +3760,13 @@
         <v>2</v>
       </c>
       <c r="O65" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="11"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="15"/>
       <c r="C66" s="3">
         <v>17</v>
       </c>
@@ -3764,21 +3795,21 @@
         <v>4</v>
       </c>
       <c r="O66" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="11"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="15"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="11"/>
+      <c r="A68" s="16"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="3">
         <v>2</v>
       </c>
@@ -3786,7 +3817,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="3">
-        <f>D68-1</f>
+        <f t="shared" ref="E68:E73" si="14">D68-1</f>
         <v>1</v>
       </c>
       <c r="F68" s="3">
@@ -3803,17 +3834,17 @@
       </c>
       <c r="K68" s="5"/>
       <c r="N68" s="6">
-        <f t="shared" ref="N68:N72" si="10">(D68-1)/$B$60</f>
+        <f t="shared" ref="N68:N72" si="15">(D68-1)/$B$60</f>
         <v>0.125</v>
       </c>
       <c r="O68" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
-      <c r="B69" s="11"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="3">
         <v>2</v>
       </c>
@@ -3821,7 +3852,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="3">
-        <f>D69-1</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F69" s="3">
@@ -3838,17 +3869,17 @@
       </c>
       <c r="K69" s="5"/>
       <c r="N69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.125</v>
       </c>
       <c r="O69" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A70" s="12"/>
-      <c r="B70" s="11"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="3">
         <v>2</v>
       </c>
@@ -3856,7 +3887,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="3">
-        <f>D70-1</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F70" s="3">
@@ -3873,17 +3904,17 @@
       </c>
       <c r="K70" s="5"/>
       <c r="N70" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.125</v>
       </c>
       <c r="O70" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A71" s="12"/>
-      <c r="B71" s="11"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="15"/>
       <c r="C71" s="3">
         <v>2</v>
       </c>
@@ -3891,7 +3922,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="3">
-        <f>D71-1</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F71" s="3">
@@ -3908,17 +3939,17 @@
       </c>
       <c r="K71" s="5"/>
       <c r="N71" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.125</v>
       </c>
       <c r="O71" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
-      <c r="B72" s="11"/>
+      <c r="A72" s="16"/>
+      <c r="B72" s="15"/>
       <c r="C72" s="3">
         <v>2</v>
       </c>
@@ -3926,7 +3957,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="3">
-        <f>D72-1</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F72" s="3">
@@ -3943,17 +3974,17 @@
       </c>
       <c r="K72" s="5"/>
       <c r="N72" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.125</v>
       </c>
       <c r="O72" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A73" s="12"/>
-      <c r="B73" s="11"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="15"/>
       <c r="C73" s="3">
         <v>2</v>
       </c>
@@ -3961,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="3">
-        <f>D73-1</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F73" s="3">
@@ -3987,8 +4018,8 @@
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
-      <c r="B74" s="11"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="15"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
@@ -4000,8 +4031,8 @@
       <c r="P74" s="10"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A75" s="12"/>
-      <c r="B75" s="11"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="15"/>
       <c r="C75" s="3">
         <v>5</v>
       </c>
@@ -4028,11 +4059,11 @@
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
       <c r="N75" s="10">
-        <f t="shared" ref="N75:N77" si="11">(D75-1)/$B$60</f>
+        <f t="shared" ref="N75:N77" si="16">(D75-1)/$B$60</f>
         <v>1</v>
       </c>
       <c r="O75" s="10">
-        <f t="shared" ref="O75:O77" si="12">F75/$B$60</f>
+        <f t="shared" ref="O75:O77" si="17">F75/$B$60</f>
         <v>1</v>
       </c>
       <c r="P75" s="4"/>
@@ -4046,8 +4077,8 @@
       <c r="X75" s="6"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
-      <c r="B76" s="11"/>
+      <c r="A76" s="16"/>
+      <c r="B76" s="15"/>
       <c r="C76" s="3">
         <v>5</v>
       </c>
@@ -4074,11 +4105,11 @@
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
       <c r="N76" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O76" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="P76" s="5"/>
@@ -4092,8 +4123,8 @@
       <c r="X76" s="6"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A77" s="12"/>
-      <c r="B77" s="11"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="3">
         <v>9</v>
       </c>
@@ -4120,11 +4151,11 @@
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
       <c r="N77" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O77" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="P77" s="4"/>
@@ -4148,10 +4179,10 @@
       <c r="O78" s="10"/>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="11">
+      <c r="B79" s="15">
         <v>3</v>
       </c>
       <c r="C79" s="3">
@@ -4183,8 +4214,8 @@
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="11"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="15"/>
       <c r="C80" s="3">
         <v>5</v>
       </c>
@@ -4192,7 +4223,7 @@
         <v>9</v>
       </c>
       <c r="E80" s="3">
-        <f t="shared" ref="E80:E98" si="13">D80-1</f>
+        <f t="shared" ref="E80:E98" si="18">D80-1</f>
         <v>8</v>
       </c>
       <c r="F80" s="3">
@@ -4214,8 +4245,8 @@
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A81" s="12"/>
-      <c r="B81" s="11"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="15"/>
       <c r="C81" s="3">
         <v>5</v>
       </c>
@@ -4223,7 +4254,7 @@
         <v>9</v>
       </c>
       <c r="E81" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F81" s="3">
@@ -4245,8 +4276,8 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A82" s="12"/>
-      <c r="B82" s="11"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="15"/>
       <c r="C82" s="3">
         <v>5</v>
       </c>
@@ -4254,7 +4285,7 @@
         <v>9</v>
       </c>
       <c r="E82" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F82" s="3">
@@ -4277,8 +4308,8 @@
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A83" s="12"/>
-      <c r="B83" s="11"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="15"/>
       <c r="C83" s="3">
         <v>9</v>
       </c>
@@ -4286,7 +4317,7 @@
         <v>17</v>
       </c>
       <c r="E83" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="F83" s="3">
@@ -4309,7 +4340,7 @@
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A84" s="12"/>
+      <c r="A84" s="16"/>
       <c r="B84" s="10"/>
       <c r="H84" s="5"/>
       <c r="I84" s="14"/>
@@ -4321,8 +4352,8 @@
       <c r="P84" s="10"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A85" s="12"/>
-      <c r="B85" s="11">
+      <c r="A85" s="16"/>
+      <c r="B85" s="15">
         <v>4</v>
       </c>
       <c r="C85" s="3">
@@ -4332,7 +4363,7 @@
         <v>5</v>
       </c>
       <c r="E85" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F85" s="3">
@@ -4345,17 +4376,17 @@
         <v>96.67</v>
       </c>
       <c r="N85" s="10">
-        <f>(D85-1)/$B$60</f>
+        <f t="shared" ref="N85:N91" si="19">(D85-1)/$B$60</f>
         <v>0.5</v>
       </c>
       <c r="O85" s="10">
-        <f>F85/$B$60</f>
+        <f t="shared" ref="O85:O91" si="20">F85/$B$60</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A86" s="12"/>
-      <c r="B86" s="11"/>
+      <c r="A86" s="16"/>
+      <c r="B86" s="15"/>
       <c r="C86" s="3">
         <v>17</v>
       </c>
@@ -4363,7 +4394,7 @@
         <v>33</v>
       </c>
       <c r="E86" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>32</v>
       </c>
       <c r="F86" s="3">
@@ -4376,17 +4407,17 @@
         <v>12.5</v>
       </c>
       <c r="N86" s="10">
-        <f>(D86-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="O86" s="10">
-        <f>F86/$B$60</f>
+        <f t="shared" si="20"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A87" s="12"/>
-      <c r="B87" s="11"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="15"/>
       <c r="C87" s="3">
         <v>5</v>
       </c>
@@ -4394,7 +4425,7 @@
         <v>9</v>
       </c>
       <c r="E87" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F87" s="3">
@@ -4407,17 +4438,17 @@
         <v>24.67</v>
       </c>
       <c r="N87" s="10">
-        <f>(D87-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="O87" s="10">
-        <f>F87/$B$60</f>
+        <f t="shared" si="20"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A88" s="12"/>
-      <c r="B88" s="11"/>
+      <c r="A88" s="16"/>
+      <c r="B88" s="15"/>
       <c r="C88" s="3">
         <v>5</v>
       </c>
@@ -4425,7 +4456,7 @@
         <v>9</v>
       </c>
       <c r="E88" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F88" s="3">
@@ -4438,17 +4469,17 @@
         <v>10.77</v>
       </c>
       <c r="N88" s="10">
-        <f>(D88-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="O88" s="10">
-        <f>F88/$B$60</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A89" s="12"/>
-      <c r="B89" s="11"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="15"/>
       <c r="C89" s="3">
         <v>5</v>
       </c>
@@ -4456,7 +4487,7 @@
         <v>9</v>
       </c>
       <c r="E89" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F89" s="3">
@@ -4469,17 +4500,17 @@
         <v>10.67</v>
       </c>
       <c r="N89" s="10">
-        <f>(D89-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="O89" s="10">
-        <f>F89/$B$60</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A90" s="12"/>
-      <c r="B90" s="11"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="15"/>
       <c r="C90" s="3">
         <v>9</v>
       </c>
@@ -4487,7 +4518,7 @@
         <v>17</v>
       </c>
       <c r="E90" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="F90" s="3">
@@ -4500,17 +4531,17 @@
         <v>5.44</v>
       </c>
       <c r="N90" s="10">
-        <f>(D90-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="O90" s="10">
-        <f>F90/$B$60</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A91" s="12"/>
-      <c r="B91" s="11"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="15"/>
       <c r="C91" s="3">
         <v>2</v>
       </c>
@@ -4518,7 +4549,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="F91" s="3">
@@ -4531,17 +4562,17 @@
         <v>83.07</v>
       </c>
       <c r="N91" s="10">
-        <f>(D91-1)/$B$60</f>
+        <f t="shared" si="19"/>
         <v>0.125</v>
       </c>
       <c r="O91" s="10">
-        <f>F91/$B$60</f>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A92" s="12"/>
-      <c r="B92" s="11"/>
+      <c r="A92" s="16"/>
+      <c r="B92" s="15"/>
       <c r="C92" s="3">
         <v>2</v>
       </c>
@@ -4549,7 +4580,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="F92" s="3">
@@ -4565,7 +4596,7 @@
       <c r="O92" s="10"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A93" s="12"/>
+      <c r="A93" s="16"/>
       <c r="B93" s="10"/>
       <c r="L93" s="10"/>
       <c r="M93" s="10"/>
@@ -4574,8 +4605,8 @@
       <c r="P93" s="10"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A94" s="12"/>
-      <c r="B94" s="11">
+      <c r="A94" s="16"/>
+      <c r="B94" s="15">
         <v>6</v>
       </c>
       <c r="C94" s="3">
@@ -4585,7 +4616,7 @@
         <v>5</v>
       </c>
       <c r="E94" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F94" s="3">
@@ -4598,17 +4629,17 @@
         <v>42.42</v>
       </c>
       <c r="N94" s="10">
-        <f t="shared" ref="N94:N98" si="14">(D94-1)/$B$60</f>
+        <f t="shared" ref="N94:N98" si="21">(D94-1)/$B$60</f>
         <v>0.5</v>
       </c>
       <c r="O94" s="10">
-        <f t="shared" ref="O94:O98" si="15">F94/$B$60</f>
+        <f t="shared" ref="O94:O98" si="22">F94/$B$60</f>
         <v>0.375</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A95" s="12"/>
-      <c r="B95" s="11"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="15"/>
       <c r="C95" s="3">
         <v>3</v>
       </c>
@@ -4616,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="E95" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F95" s="3">
@@ -4629,17 +4660,17 @@
         <v>20.25</v>
       </c>
       <c r="N95" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
       <c r="O95" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0.625</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A96" s="12"/>
-      <c r="B96" s="11"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="15"/>
       <c r="C96" s="3">
         <v>3</v>
       </c>
@@ -4647,7 +4678,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="F96" s="3">
@@ -4660,17 +4691,17 @@
         <v>20.49</v>
       </c>
       <c r="N96" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
       <c r="O96" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A97" s="12"/>
-      <c r="B97" s="11"/>
+      <c r="A97" s="16"/>
+      <c r="B97" s="15"/>
       <c r="C97" s="3">
         <v>5</v>
       </c>
@@ -4678,7 +4709,7 @@
         <v>10</v>
       </c>
       <c r="E97" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="F97" s="3">
@@ -4691,17 +4722,17 @@
         <v>19.7</v>
       </c>
       <c r="N97" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>1.125</v>
       </c>
       <c r="O97" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0.625</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A98" s="12"/>
-      <c r="B98" s="11"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="15"/>
       <c r="C98" s="3">
         <v>6</v>
       </c>
@@ -4709,7 +4740,7 @@
         <v>12</v>
       </c>
       <c r="E98" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="F98" s="3">
@@ -4722,11 +4753,11 @@
         <v>16.309999999999999</v>
       </c>
       <c r="N98" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>1.375</v>
       </c>
       <c r="O98" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>0.625</v>
       </c>
     </row>
@@ -4745,4 +4776,881 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1587C65C-2A02-40EA-881D-83CE6FB2DC91}">
+  <dimension ref="A1:L40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2-1</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I2" s="18">
+        <v>39.25</v>
+      </c>
+      <c r="J2" s="1">
+        <v>26.4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>19.64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3-1</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I3" s="18">
+        <v>39.93</v>
+      </c>
+      <c r="J3" s="1">
+        <v>22.07</v>
+      </c>
+      <c r="K3" s="1">
+        <v>19.75</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4-1</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I4" s="18">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="J4" s="1">
+        <v>26.73</v>
+      </c>
+      <c r="K4" s="1">
+        <v>19.63</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6-1</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I6" s="18">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1">
+        <v>12.22</v>
+      </c>
+      <c r="K6" s="1">
+        <v>10.64</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7-1</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I7" s="18">
+        <v>6.01</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8.89</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5.63</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8-1</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I8" s="18">
+        <v>12.63</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8.93</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5.65</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E12" si="0">D10-1</f>
+        <v>6</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I10" s="18">
+        <v>6.39</v>
+      </c>
+      <c r="J10" s="1">
+        <v>6.33</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5.31</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I11" s="18">
+        <v>5.53</v>
+      </c>
+      <c r="J11" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="3">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="I12" s="18">
+        <v>6.46</v>
+      </c>
+      <c r="J12" s="1">
+        <v>6.48</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5.39</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f>D15-1</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="J15" s="1">
+        <v>61.4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>33.56</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <f>D16-1</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="J16" s="1">
+        <v>31.82</v>
+      </c>
+      <c r="K16" s="1">
+        <v>17.43</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <f>D17-1</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>16</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18">
+        <v>11.45</v>
+      </c>
+      <c r="J17" s="1">
+        <v>18.18</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3">
+        <f>D19-1</f>
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18">
+        <v>12.58</v>
+      </c>
+      <c r="J19" s="1">
+        <v>21.79</v>
+      </c>
+      <c r="K19" s="1">
+        <v>12.14</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <f>D20-1</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18">
+        <v>7.9</v>
+      </c>
+      <c r="J20" s="1">
+        <v>12.13</v>
+      </c>
+      <c r="K20" s="1">
+        <v>6.82</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3">
+        <f>D21-1</f>
+        <v>3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>16</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18">
+        <v>6.88</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6.43</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5.26</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" ref="E23:E25" si="1">D23-1</f>
+        <v>6</v>
+      </c>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18">
+        <v>6.55</v>
+      </c>
+      <c r="J23" s="1">
+        <v>11.34</v>
+      </c>
+      <c r="K23" s="1">
+        <v>6.61</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F24" s="3">
+        <v>8</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18">
+        <v>10.32</v>
+      </c>
+      <c r="J24" s="1">
+        <v>6.21</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4.08</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F25" s="3">
+        <v>16</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18">
+        <v>5.53</v>
+      </c>
+      <c r="J25" s="1">
+        <v>3.93</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3.01</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="A2:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
determine threadsPerBlock & set GPU work proportion to 0.75
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LM2P\Documents\000_TTU_UT\Euroteq\Distributed &amp; Parallel Computing\apm\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBC12C-2E6C-4454-9AC7-8E0B5268DACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28721DE-A69B-4007-B5E7-388E26FCE5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DE9C4FAA-FE23-4741-8F2C-7B77D437BC47}"/>
   </bookViews>
   <sheets>
     <sheet name="Hybrid - No GPU" sheetId="1" r:id="rId1"/>
     <sheet name="With GPU" sheetId="2" r:id="rId2"/>
+    <sheet name="threadsPerBlock determination" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E8295813-83C2-41ED-AF3F-86E50477CE93}</author>
+    <author>tc={A9A4E289-D2BA-405F-AAA3-8B6F18C3F3E1}</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{E8295813-83C2-41ED-AF3F-86E50477CE93}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Worst case scenario</t>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="1" shapeId="0" xr:uid="{A9A4E289-D2BA-405F-AAA3-8B6F18C3F3E1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maximum threads per block in Quadro P2000</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t># Nodes</t>
   </si>
@@ -121,12 +149,27 @@
   <si>
     <t>Levenshtein Computation Executed</t>
   </si>
+  <si>
+    <t>threadsPerBlock</t>
+  </si>
+  <si>
+    <t>Avg. Duration of ComputeMatches Kernel  - GPU taking 50% of job  [s]</t>
+  </si>
+  <si>
+    <t>Avg. Duration of ComputeMatches Kernel - GPU taking 75% of job [s]</t>
+  </si>
+  <si>
+    <t>Patterns-over-ranks execution time - GPU taking 50% of job  [s]</t>
+  </si>
+  <si>
+    <t>Patterns-over-ranks execution time - GPU taking 75% of job  [s]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +177,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,6 +264,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1323,6 +1417,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Lino Mediavilla" id="{DA869B71-6C02-47EC-943F-6AD47E341FF3}" userId="8911ff9ca497036c" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1618,6 +1718,17 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A2" dT="2022-03-17T03:41:55.16" personId="{DA869B71-6C02-47EC-943F-6AD47E341FF3}" id="{E8295813-83C2-41ED-AF3F-86E50477CE93}">
+    <text>Worst case scenario</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2022-03-17T03:41:30.60" personId="{DA869B71-6C02-47EC-943F-6AD47E341FF3}" id="{A9A4E289-D2BA-405F-AAA3-8B6F18C3F3E1}">
+    <text>Maximum threads per block in Quadro P2000</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5605-5B40-4E95-A326-20DE76CB0444}">
   <dimension ref="A1:X98"/>
@@ -1693,10 +1804,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="19">
         <v>1</v>
       </c>
       <c r="C2" s="3">
@@ -1744,16 +1855,16 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="19"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -1805,8 +1916,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="3">
         <v>3</v>
       </c>
@@ -1852,8 +1963,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1899,8 +2010,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="3">
         <v>9</v>
       </c>
@@ -1949,8 +2060,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="3">
         <v>17</v>
       </c>
@@ -1999,16 +2110,16 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="19"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="3">
         <v>2</v>
       </c>
@@ -2054,8 +2165,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -2101,8 +2212,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="3">
         <v>2</v>
       </c>
@@ -2148,8 +2259,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="3">
         <v>2</v>
       </c>
@@ -2195,8 +2306,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="3">
         <v>2</v>
       </c>
@@ -2242,8 +2353,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="3">
         <v>2</v>
       </c>
@@ -2289,8 +2400,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="19"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2302,8 +2413,8 @@
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="3">
         <v>5</v>
       </c>
@@ -2340,8 +2451,8 @@
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="3">
         <v>5</v>
       </c>
@@ -2378,8 +2489,8 @@
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="3">
         <v>9</v>
       </c>
@@ -2416,7 +2527,7 @@
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="10"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2429,15 +2540,15 @@
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+      <c r="A21" s="20"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15">
+      <c r="A22" s="20"/>
+      <c r="B22" s="19">
         <v>2</v>
       </c>
       <c r="C22" s="3">
@@ -2473,16 +2584,16 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="19"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="3">
         <v>2</v>
       </c>
@@ -2516,8 +2627,8 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="3">
         <v>3</v>
       </c>
@@ -2551,8 +2662,8 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="3">
         <v>5</v>
       </c>
@@ -2586,8 +2697,8 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3">
         <v>9</v>
       </c>
@@ -2621,8 +2732,8 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3">
         <v>17</v>
       </c>
@@ -2656,16 +2767,16 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="19"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="3">
         <v>2</v>
       </c>
@@ -2699,8 +2810,8 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="3">
         <v>2</v>
       </c>
@@ -2734,8 +2845,8 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="3">
         <v>2</v>
       </c>
@@ -2769,8 +2880,8 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="3">
         <v>2</v>
       </c>
@@ -2804,8 +2915,8 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="3">
         <v>2</v>
       </c>
@@ -2839,8 +2950,8 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="3">
         <v>2</v>
       </c>
@@ -2874,8 +2985,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="19"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -2887,8 +2998,8 @@
       <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="15"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="3">
         <v>5</v>
       </c>
@@ -2925,8 +3036,8 @@
       <c r="P37" s="10"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="3">
         <v>5</v>
       </c>
@@ -2963,8 +3074,8 @@
       <c r="P38" s="10"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="15"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="3">
         <v>9</v>
       </c>
@@ -3001,15 +3112,15 @@
       <c r="P39" s="10"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
+      <c r="A40" s="20"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="15">
+      <c r="A41" s="20"/>
+      <c r="B41" s="19">
         <v>4</v>
       </c>
       <c r="C41" s="3">
@@ -3045,16 +3156,16 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="15"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="3">
         <v>2</v>
       </c>
@@ -3088,8 +3199,8 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="3">
         <v>3</v>
       </c>
@@ -3123,8 +3234,8 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="3">
         <v>5</v>
       </c>
@@ -3158,8 +3269,8 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="3">
         <v>9</v>
       </c>
@@ -3193,8 +3304,8 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="3">
         <v>17</v>
       </c>
@@ -3228,16 +3339,16 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="19"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="15"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="19"/>
       <c r="C49" s="3">
         <v>2</v>
       </c>
@@ -3271,8 +3382,8 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="3">
         <v>2</v>
       </c>
@@ -3306,8 +3417,8 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="16"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="19"/>
       <c r="C51" s="3">
         <v>2</v>
       </c>
@@ -3341,8 +3452,8 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="20"/>
+      <c r="B52" s="19"/>
       <c r="C52" s="3">
         <v>2</v>
       </c>
@@ -3376,8 +3487,8 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A53" s="16"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="3">
         <v>2</v>
       </c>
@@ -3411,8 +3522,8 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="15"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="19"/>
       <c r="C54" s="3">
         <v>2</v>
       </c>
@@ -3446,8 +3557,8 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="15"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="19"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -3459,8 +3570,8 @@
       <c r="P55" s="10"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="15"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="19"/>
       <c r="C56" s="3">
         <v>5</v>
       </c>
@@ -3497,8 +3608,8 @@
       <c r="P56" s="10"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="16"/>
-      <c r="B57" s="15"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="19"/>
       <c r="C57" s="3">
         <v>5</v>
       </c>
@@ -3535,8 +3646,8 @@
       <c r="P57" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="16"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="19"/>
       <c r="C58" s="3">
         <v>9</v>
       </c>
@@ -3573,15 +3684,15 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="16"/>
+      <c r="A59" s="20"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="16"/>
-      <c r="B60" s="15">
+      <c r="A60" s="20"/>
+      <c r="B60" s="19">
         <v>8</v>
       </c>
       <c r="C60" s="3">
@@ -3617,16 +3728,16 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="16"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="19"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="16"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="3">
         <v>2</v>
       </c>
@@ -3660,8 +3771,8 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="16"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="3">
         <v>3</v>
       </c>
@@ -3695,8 +3806,8 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="16"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="3">
         <v>5</v>
       </c>
@@ -3730,8 +3841,8 @@
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A65" s="16"/>
-      <c r="B65" s="15"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="19"/>
       <c r="C65" s="3">
         <v>9</v>
       </c>
@@ -3765,8 +3876,8 @@
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A66" s="16"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="3">
         <v>17</v>
       </c>
@@ -3800,16 +3911,16 @@
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A67" s="16"/>
-      <c r="B67" s="15"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="19"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
-      <c r="B68" s="15"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="19"/>
       <c r="C68" s="3">
         <v>2</v>
       </c>
@@ -3843,8 +3954,8 @@
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
-      <c r="B69" s="15"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="19"/>
       <c r="C69" s="3">
         <v>2</v>
       </c>
@@ -3878,8 +3989,8 @@
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
-      <c r="B70" s="15"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="3">
         <v>2</v>
       </c>
@@ -3913,8 +4024,8 @@
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
-      <c r="B71" s="15"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="19"/>
       <c r="C71" s="3">
         <v>2</v>
       </c>
@@ -3948,8 +4059,8 @@
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
-      <c r="B72" s="15"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="19"/>
       <c r="C72" s="3">
         <v>2</v>
       </c>
@@ -3983,8 +4094,8 @@
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A73" s="16"/>
-      <c r="B73" s="15"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="19"/>
       <c r="C73" s="3">
         <v>2</v>
       </c>
@@ -4018,8 +4129,8 @@
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A74" s="16"/>
-      <c r="B74" s="15"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="19"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
@@ -4031,8 +4142,8 @@
       <c r="P74" s="10"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A75" s="16"/>
-      <c r="B75" s="15"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="3">
         <v>5</v>
       </c>
@@ -4077,8 +4188,8 @@
       <c r="X75" s="6"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A76" s="16"/>
-      <c r="B76" s="15"/>
+      <c r="A76" s="20"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="3">
         <v>5</v>
       </c>
@@ -4123,8 +4234,8 @@
       <c r="X76" s="6"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A77" s="16"/>
-      <c r="B77" s="15"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="3">
         <v>9</v>
       </c>
@@ -4179,10 +4290,10 @@
       <c r="O78" s="10"/>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="15">
+      <c r="B79" s="19">
         <v>3</v>
       </c>
       <c r="C79" s="3">
@@ -4214,8 +4325,8 @@
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A80" s="16"/>
-      <c r="B80" s="15"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="19"/>
       <c r="C80" s="3">
         <v>5</v>
       </c>
@@ -4245,8 +4356,8 @@
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A81" s="16"/>
-      <c r="B81" s="15"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="19"/>
       <c r="C81" s="3">
         <v>5</v>
       </c>
@@ -4276,8 +4387,8 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A82" s="16"/>
-      <c r="B82" s="15"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="3">
         <v>5</v>
       </c>
@@ -4308,8 +4419,8 @@
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A83" s="16"/>
-      <c r="B83" s="15"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="19"/>
       <c r="C83" s="3">
         <v>9</v>
       </c>
@@ -4340,7 +4451,7 @@
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A84" s="16"/>
+      <c r="A84" s="20"/>
       <c r="B84" s="10"/>
       <c r="H84" s="5"/>
       <c r="I84" s="14"/>
@@ -4352,8 +4463,8 @@
       <c r="P84" s="10"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A85" s="16"/>
-      <c r="B85" s="15">
+      <c r="A85" s="20"/>
+      <c r="B85" s="19">
         <v>4</v>
       </c>
       <c r="C85" s="3">
@@ -4385,8 +4496,8 @@
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A86" s="16"/>
-      <c r="B86" s="15"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="19"/>
       <c r="C86" s="3">
         <v>17</v>
       </c>
@@ -4416,8 +4527,8 @@
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A87" s="16"/>
-      <c r="B87" s="15"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="19"/>
       <c r="C87" s="3">
         <v>5</v>
       </c>
@@ -4447,8 +4558,8 @@
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A88" s="16"/>
-      <c r="B88" s="15"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="19"/>
       <c r="C88" s="3">
         <v>5</v>
       </c>
@@ -4478,8 +4589,8 @@
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A89" s="16"/>
-      <c r="B89" s="15"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="19"/>
       <c r="C89" s="3">
         <v>5</v>
       </c>
@@ -4509,8 +4620,8 @@
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A90" s="16"/>
-      <c r="B90" s="15"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="19"/>
       <c r="C90" s="3">
         <v>9</v>
       </c>
@@ -4540,8 +4651,8 @@
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A91" s="16"/>
-      <c r="B91" s="15"/>
+      <c r="A91" s="20"/>
+      <c r="B91" s="19"/>
       <c r="C91" s="3">
         <v>2</v>
       </c>
@@ -4571,8 +4682,8 @@
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A92" s="16"/>
-      <c r="B92" s="15"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="19"/>
       <c r="C92" s="3">
         <v>2</v>
       </c>
@@ -4596,7 +4707,7 @@
       <c r="O92" s="10"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A93" s="16"/>
+      <c r="A93" s="20"/>
       <c r="B93" s="10"/>
       <c r="L93" s="10"/>
       <c r="M93" s="10"/>
@@ -4605,8 +4716,8 @@
       <c r="P93" s="10"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A94" s="16"/>
-      <c r="B94" s="15">
+      <c r="A94" s="20"/>
+      <c r="B94" s="19">
         <v>6</v>
       </c>
       <c r="C94" s="3">
@@ -4638,8 +4749,8 @@
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A95" s="16"/>
-      <c r="B95" s="15"/>
+      <c r="A95" s="20"/>
+      <c r="B95" s="19"/>
       <c r="C95" s="3">
         <v>3</v>
       </c>
@@ -4669,8 +4780,8 @@
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A96" s="16"/>
-      <c r="B96" s="15"/>
+      <c r="A96" s="20"/>
+      <c r="B96" s="19"/>
       <c r="C96" s="3">
         <v>3</v>
       </c>
@@ -4700,8 +4811,8 @@
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A97" s="16"/>
-      <c r="B97" s="15"/>
+      <c r="A97" s="20"/>
+      <c r="B97" s="19"/>
       <c r="C97" s="3">
         <v>5</v>
       </c>
@@ -4731,8 +4842,8 @@
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A98" s="16"/>
-      <c r="B98" s="15"/>
+      <c r="A98" s="20"/>
+      <c r="B98" s="19"/>
       <c r="C98" s="3">
         <v>6</v>
       </c>
@@ -4783,7 +4894,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4836,10 +4947,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="19">
         <v>6</v>
       </c>
       <c r="C2" s="3">
@@ -4873,8 +4984,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3">
         <v>1</v>
       </c>
@@ -4906,8 +5017,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -4939,8 +5050,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -4950,8 +5061,8 @@
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="3">
         <v>2</v>
       </c>
@@ -4983,8 +5094,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -5002,22 +5113,22 @@
       <c r="H7" s="18">
         <v>49.5</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="28">
         <v>6.01</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="29">
         <v>8.89</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="29">
         <v>5.63</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="29" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="3">
         <v>2</v>
       </c>
@@ -5049,8 +5160,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -5060,8 +5171,8 @@
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="3">
         <v>3</v>
       </c>
@@ -5093,8 +5204,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="3">
         <v>3</v>
       </c>
@@ -5126,8 +5237,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -5159,8 +5270,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -5170,8 +5281,8 @@
       <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -5181,8 +5292,8 @@
       <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="3">
         <v>1</v>
       </c>
@@ -5212,8 +5323,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="3">
         <v>1</v>
       </c>
@@ -5243,8 +5354,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="3">
         <v>1</v>
       </c>
@@ -5274,8 +5385,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5285,8 +5396,8 @@
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="3">
         <v>2</v>
       </c>
@@ -5316,8 +5427,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="3">
         <v>2</v>
       </c>
@@ -5347,8 +5458,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="3">
         <v>2</v>
       </c>
@@ -5378,8 +5489,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -5389,8 +5500,8 @@
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="3">
         <v>3</v>
       </c>
@@ -5420,8 +5531,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="3">
         <v>3</v>
       </c>
@@ -5451,8 +5562,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="3">
         <v>3</v>
       </c>
@@ -5653,4 +5764,304 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517EFAF9-8FE3-43A9-BD7C-E66B852BDA31}">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="16.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="19">
+        <v>6</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21">
+        <v>1024</v>
+      </c>
+      <c r="G2" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="H2" s="23">
+        <v>41.396999999999998</v>
+      </c>
+      <c r="I2" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="J2" s="23">
+        <v>26.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="1">
+        <v>512</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="H3" s="23">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="I3" s="23">
+        <v>1.84</v>
+      </c>
+      <c r="J3" s="23">
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="1">
+        <v>256</v>
+      </c>
+      <c r="G4" s="23">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H4" s="23">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1.58</v>
+      </c>
+      <c r="J4" s="23">
+        <v>25.07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="26">
+        <v>128</v>
+      </c>
+      <c r="G5" s="27">
+        <f>967.48/1000</f>
+        <v>0.96748000000000001</v>
+      </c>
+      <c r="H5" s="27">
+        <v>37.86</v>
+      </c>
+      <c r="I5" s="27">
+        <v>1.24</v>
+      </c>
+      <c r="J5" s="27">
+        <v>23.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="1">
+        <v>96</v>
+      </c>
+      <c r="G6" s="23">
+        <f>936.99/1000</f>
+        <v>0.93698999999999999</v>
+      </c>
+      <c r="H6" s="23">
+        <v>37.61</v>
+      </c>
+      <c r="I6" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="J6" s="23">
+        <v>24.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="1">
+        <v>64</v>
+      </c>
+      <c r="G7" s="23">
+        <v>1.0000260000000001</v>
+      </c>
+      <c r="H7" s="23">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="I7" s="23">
+        <v>1.38</v>
+      </c>
+      <c r="J7" s="23">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="24">
+        <v>32</v>
+      </c>
+      <c r="G8" s="25">
+        <f>542/1000</f>
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="H8" s="25">
+        <v>35.01</v>
+      </c>
+      <c r="I8" s="25">
+        <f>739.57/1000</f>
+        <v>0.73957000000000006</v>
+      </c>
+      <c r="J8" s="25">
+        <v>20.149999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>